<commit_message>
excel helper and driver files
</commit_message>
<xml_diff>
--- a/resources/input.xlsx
+++ b/resources/input.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="5535" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="testcases" sheetId="1" r:id="rId1"/>
     <sheet name="teststeps" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="59">
   <si>
     <t>Test case ID</t>
   </si>
@@ -47,9 +47,6 @@
     <t>branch creation with valid data</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>TC_logout_004</t>
   </si>
   <si>
@@ -189,6 +186,12 @@
   </si>
   <si>
     <t>closeBrowser</t>
+  </si>
+  <si>
+    <t>click on branch button</t>
+  </si>
+  <si>
+    <t>img[src *= 'Branches']</t>
   </si>
 </sst>
 </file>
@@ -553,7 +556,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,15 +606,15 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
         <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -625,15 +628,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.85546875" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" customWidth="1"/>
@@ -646,19 +649,19 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -666,13 +669,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -680,13 +683,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
         <v>21</v>
       </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -694,19 +697,19 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
         <v>25</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>26</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>27</v>
-      </c>
-      <c r="F4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -714,19 +717,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
         <v>29</v>
       </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>30</v>
-      </c>
       <c r="E5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" t="s">
         <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -734,16 +737,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
         <v>31</v>
       </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>32</v>
-      </c>
-      <c r="E6" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -751,10 +754,10 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
         <v>34</v>
-      </c>
-      <c r="E7" t="s">
-        <v>35</v>
       </c>
       <c r="F7">
         <v>5000</v>
@@ -765,16 +768,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" t="s">
         <v>36</v>
       </c>
-      <c r="C8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" t="s">
-        <v>37</v>
-      </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -782,16 +785,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
         <v>39</v>
       </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" t="s">
-        <v>40</v>
-      </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -799,19 +802,19 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
         <v>41</v>
       </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" t="s">
         <v>42</v>
-      </c>
-      <c r="E10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -819,19 +822,19 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>45</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>46</v>
-      </c>
-      <c r="F11" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -839,16 +842,16 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" t="s">
         <v>48</v>
       </c>
-      <c r="C12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" t="s">
-        <v>49</v>
-      </c>
       <c r="E12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -856,10 +859,10 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" t="s">
         <v>50</v>
-      </c>
-      <c r="E13" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -867,10 +870,10 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" t="s">
         <v>52</v>
-      </c>
-      <c r="E14" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -878,10 +881,10 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" t="s">
         <v>34</v>
-      </c>
-      <c r="E15" t="s">
-        <v>35</v>
       </c>
       <c r="F15">
         <v>5000</v>
@@ -889,30 +892,47 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" t="s">
         <v>54</v>
       </c>
-      <c r="C16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" t="s">
-        <v>55</v>
-      </c>
       <c r="E16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" t="s">
         <v>56</v>
       </c>
-      <c r="E17" t="s">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" t="s">
         <v>57</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>